<commit_message>
Larvaledamos con errores losiento :)
</commit_message>
<xml_diff>
--- a/01 - Planificación del Trabajo/estadisticoHorasEmpleadas.xlsx
+++ b/01 - Planificación del Trabajo/estadisticoHorasEmpleadas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrés Martín Yeves\Desktop\TP1\SE\TP1SE\01 - Planificación del Trabajo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0389413A-427A-435B-B809-BCAD2DE3E4D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD0A765-35AF-43CE-9A2B-1438CBBD8EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E923A452-E286-4F7D-AF6D-30DFC2805F3A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>Número de Horas empleadas por los trabajadores:</t>
   </si>
@@ -124,13 +124,13 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -362,6 +362,18 @@
                 <c:pt idx="49">
                   <c:v>1.5</c:v>
                 </c:pt>
+                <c:pt idx="61">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.65</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -447,6 +459,21 @@
                 <c:pt idx="60">
                   <c:v>0.75</c:v>
                 </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.65</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -526,6 +553,18 @@
                 <c:pt idx="49">
                   <c:v>1.5</c:v>
                 </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.65</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.75</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -613,6 +652,21 @@
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.65</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1732,10 +1786,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A57A6FB7-D46D-488C-A966-0ADB5C61A67C}">
-  <dimension ref="E2:L143"/>
+  <dimension ref="E1:L143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B123" zoomScale="99" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="99" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="H77" sqref="H77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1744,22 +1800,39 @@
     <col min="4" max="6" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="2" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E2" s="1"/>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="5:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E3" s="1"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="5:10" x14ac:dyDescent="0.3">
@@ -2348,7 +2421,7 @@
       <c r="G64" s="4"/>
       <c r="H64" s="4"/>
     </row>
-    <row r="65" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F65" s="3">
         <v>44886</v>
       </c>
@@ -2357,105 +2430,150 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="66" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F66" s="3">
         <v>44887</v>
       </c>
-      <c r="G66" s="4"/>
-      <c r="H66" s="4"/>
-    </row>
-    <row r="67" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="G66" s="4">
+        <v>2.6</v>
+      </c>
+      <c r="H66" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="I66">
+        <v>1.3</v>
+      </c>
+      <c r="J66">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="67" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F67" s="3">
         <v>44888</v>
       </c>
       <c r="G67" s="4"/>
       <c r="H67" s="4"/>
-    </row>
-    <row r="68" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="J67">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="68" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F68" s="3">
         <v>44889</v>
       </c>
-      <c r="G68" s="4"/>
-      <c r="H68" s="4"/>
-    </row>
-    <row r="69" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="G68" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="H68" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="I68">
+        <v>3.5</v>
+      </c>
+      <c r="J68">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="69" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F69" s="3">
         <v>44890</v>
       </c>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
     </row>
-    <row r="70" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F70" s="3">
         <v>44891</v>
       </c>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
     </row>
-    <row r="71" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F71" s="3">
         <v>44892</v>
       </c>
-      <c r="G71" s="4"/>
+      <c r="G71" s="4">
+        <v>1.5</v>
+      </c>
       <c r="H71" s="4"/>
     </row>
-    <row r="72" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F72" s="3">
         <v>44893</v>
       </c>
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
     </row>
-    <row r="73" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F73" s="3">
         <v>44894</v>
       </c>
-      <c r="G73" s="4"/>
-      <c r="H73" s="4"/>
-    </row>
-    <row r="74" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="G73" s="4">
+        <v>1.65</v>
+      </c>
+      <c r="H73" s="4">
+        <v>1.65</v>
+      </c>
+      <c r="I73">
+        <v>1.65</v>
+      </c>
+      <c r="J73">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="74" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F74" s="3">
         <v>44895</v>
       </c>
       <c r="G74" s="4"/>
       <c r="H74" s="4"/>
     </row>
-    <row r="75" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F75" s="3">
         <v>44896</v>
       </c>
       <c r="G75" s="4"/>
-      <c r="H75" s="4"/>
-    </row>
-    <row r="76" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="H75" s="4">
+        <v>1.75</v>
+      </c>
+      <c r="I75">
+        <v>1.75</v>
+      </c>
+      <c r="J75">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="76" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F76" s="3">
         <v>44897</v>
       </c>
       <c r="G76" s="4"/>
       <c r="H76" s="4"/>
     </row>
-    <row r="77" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F77" s="3">
         <v>44898</v>
       </c>
       <c r="G77" s="4"/>
       <c r="H77" s="4"/>
     </row>
-    <row r="78" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F78" s="3">
         <v>44899</v>
       </c>
       <c r="G78" s="4"/>
-      <c r="H78" s="4"/>
-    </row>
-    <row r="79" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="H78" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F79" s="3">
         <v>44900</v>
       </c>
       <c r="G79" s="4"/>
       <c r="H79" s="4"/>
     </row>
-    <row r="80" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F80" s="3">
         <v>44901</v>
       </c>
@@ -2851,38 +2969,38 @@
       <c r="F138" s="3"/>
     </row>
     <row r="139" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E139" s="7" t="s">
+      <c r="E139" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F139" s="7"/>
-      <c r="G139" s="8">
+      <c r="F139" s="8"/>
+      <c r="G139" s="6">
         <f>SUM(G5,G5:G137)</f>
-        <v>23</v>
-      </c>
-      <c r="H139" s="8">
+        <v>30.25</v>
+      </c>
+      <c r="H139" s="6">
         <f>SUM(H5,H6:H138)</f>
-        <v>20.65</v>
-      </c>
-      <c r="I139" s="8">
+        <v>27.849999999999998</v>
+      </c>
+      <c r="I139" s="6">
         <f>SUM(I5,I6:I138)</f>
-        <v>15.9</v>
-      </c>
-      <c r="J139" s="8">
+        <v>24.099999999999998</v>
+      </c>
+      <c r="J139" s="6">
         <f>SUM(J5,J6:J138)</f>
-        <v>26</v>
-      </c>
-      <c r="L139" s="8" t="s">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="L139" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="140" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E140" s="7"/>
-      <c r="F140" s="7"/>
-      <c r="G140" s="8"/>
-      <c r="H140" s="8"/>
-      <c r="I140" s="8"/>
-      <c r="J140" s="8"/>
-      <c r="L140" s="8"/>
+      <c r="E140" s="8"/>
+      <c r="F140" s="8"/>
+      <c r="G140" s="6"/>
+      <c r="H140" s="6"/>
+      <c r="I140" s="6"/>
+      <c r="J140" s="6"/>
+      <c r="L140" s="6"/>
     </row>
     <row r="141" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E141" s="9" t="s">
@@ -2901,50 +3019,45 @@
       <c r="J141" s="5">
         <v>15.625</v>
       </c>
-      <c r="L141" s="8"/>
+      <c r="L141" s="6"/>
     </row>
     <row r="142" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E142" s="8" t="s">
+      <c r="E142" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F142" s="8"/>
-      <c r="G142" s="8">
+      <c r="F142" s="6"/>
+      <c r="G142" s="6">
         <f>PRODUCT(G139,G141)</f>
-        <v>359.375</v>
-      </c>
-      <c r="H142" s="8">
+        <v>472.65625</v>
+      </c>
+      <c r="H142" s="6">
         <f>PRODUCT(H139,H141)</f>
-        <v>322.65625</v>
-      </c>
-      <c r="I142" s="8">
+        <v>435.15624999999994</v>
+      </c>
+      <c r="I142" s="6">
         <f t="shared" ref="I142:J142" si="0">PRODUCT(I139,I141)</f>
-        <v>248.4375</v>
-      </c>
-      <c r="J142" s="8">
+        <v>376.56249999999994</v>
+      </c>
+      <c r="J142" s="6">
         <f t="shared" si="0"/>
-        <v>406.25</v>
-      </c>
-      <c r="L142" s="8">
+        <v>550</v>
+      </c>
+      <c r="L142" s="6">
         <f>SUM(G142:J143)</f>
-        <v>1336.71875</v>
+        <v>1834.375</v>
       </c>
     </row>
     <row r="143" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E143" s="8"/>
-      <c r="F143" s="8"/>
-      <c r="G143" s="8"/>
-      <c r="H143" s="8"/>
-      <c r="I143" s="8"/>
-      <c r="J143" s="8"/>
-      <c r="L143" s="8"/>
+      <c r="E143" s="6"/>
+      <c r="F143" s="6"/>
+      <c r="G143" s="6"/>
+      <c r="H143" s="6"/>
+      <c r="I143" s="6"/>
+      <c r="J143" s="6"/>
+      <c r="L143" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="L139:L141"/>
-    <mergeCell ref="L142:L143"/>
-    <mergeCell ref="I139:I140"/>
-    <mergeCell ref="J139:J140"/>
-    <mergeCell ref="J142:J143"/>
     <mergeCell ref="F2:I3"/>
     <mergeCell ref="E139:F140"/>
     <mergeCell ref="G139:G140"/>
@@ -2954,6 +3067,11 @@
     <mergeCell ref="H142:H143"/>
     <mergeCell ref="E141:F141"/>
     <mergeCell ref="I142:I143"/>
+    <mergeCell ref="L139:L141"/>
+    <mergeCell ref="L142:L143"/>
+    <mergeCell ref="I139:I140"/>
+    <mergeCell ref="J139:J140"/>
+    <mergeCell ref="J142:J143"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualizacion Estadistico y control de cambios
</commit_message>
<xml_diff>
--- a/01 - Planificación del Trabajo/estadisticoHorasEmpleadas.xlsx
+++ b/01 - Planificación del Trabajo/estadisticoHorasEmpleadas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrés Martín Yeves\Desktop\TP1\SE\TP1SE\01 - Planificación del Trabajo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D40141D-0348-40C5-AB71-983FEF25C74A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E8F0C4-4C56-4EC1-A207-D058FCEF7493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E923A452-E286-4F7D-AF6D-30DFC2805F3A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E923A452-E286-4F7D-AF6D-30DFC2805F3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -124,13 +124,13 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -343,6 +343,21 @@
                 <c:pt idx="82">
                   <c:v>1.5</c:v>
                 </c:pt>
+                <c:pt idx="84">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -445,6 +460,18 @@
                 <c:pt idx="82">
                   <c:v>1.5</c:v>
                 </c:pt>
+                <c:pt idx="84">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -544,6 +571,15 @@
                 <c:pt idx="82">
                   <c:v>1.5</c:v>
                 </c:pt>
+                <c:pt idx="89">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -659,6 +695,24 @@
                   <c:v>4.6500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="82">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>4.25</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="92">
                   <c:v>1.5</c:v>
                 </c:pt>
               </c:numCache>
@@ -1741,9 +1795,9 @@
   <dimension ref="E1:L143"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
+      <selection pane="bottomLeft" activeCell="K133" sqref="K133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1771,20 +1825,20 @@
     </row>
     <row r="2" spans="5:10" x14ac:dyDescent="0.3">
       <c r="E2" s="1"/>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="5:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E3" s="1"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="5:10" x14ac:dyDescent="0.3">
@@ -2624,15 +2678,27 @@
       <c r="F89" s="3">
         <v>44910</v>
       </c>
-      <c r="G89" s="4"/>
-      <c r="H89" s="4"/>
+      <c r="G89" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="H89" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="J89">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="90" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F90" s="3">
         <v>44911</v>
       </c>
-      <c r="G90" s="4"/>
+      <c r="G90" s="4">
+        <v>2</v>
+      </c>
       <c r="H90" s="4"/>
+      <c r="J90">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="91" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F91" s="3">
@@ -2659,129 +2725,162 @@
       <c r="F94" s="3">
         <v>44915</v>
       </c>
-      <c r="G94" s="4"/>
-      <c r="H94" s="4"/>
+      <c r="G94" s="4">
+        <v>2</v>
+      </c>
+      <c r="H94" s="4">
+        <v>2</v>
+      </c>
+      <c r="I94">
+        <v>2</v>
+      </c>
+      <c r="J94">
+        <v>3</v>
+      </c>
     </row>
     <row r="95" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F95" s="3">
         <v>44916</v>
       </c>
       <c r="G95" s="4"/>
-      <c r="H95" s="4"/>
+      <c r="H95" s="4">
+        <v>2.75</v>
+      </c>
+      <c r="I95">
+        <v>1.75</v>
+      </c>
+      <c r="J95">
+        <v>4.25</v>
+      </c>
     </row>
     <row r="96" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F96" s="3">
         <v>44917</v>
       </c>
-      <c r="G96" s="4"/>
-      <c r="H96" s="4"/>
-    </row>
-    <row r="97" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="G96" s="4">
+        <v>2</v>
+      </c>
+      <c r="H96" s="4">
+        <v>2</v>
+      </c>
+      <c r="I96">
+        <v>2</v>
+      </c>
+      <c r="J96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F97" s="3">
         <v>44918</v>
       </c>
-      <c r="G97" s="4"/>
+      <c r="G97" s="4">
+        <v>2.5</v>
+      </c>
       <c r="H97" s="4"/>
-    </row>
-    <row r="98" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="J97">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="98" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F98" s="3">
         <v>44919</v>
       </c>
       <c r="G98" s="4"/>
       <c r="H98" s="4"/>
     </row>
-    <row r="99" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F99" s="3">
         <v>44920</v>
       </c>
       <c r="G99" s="4"/>
       <c r="H99" s="4"/>
     </row>
-    <row r="100" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F100" s="3">
         <v>44921</v>
       </c>
       <c r="G100" s="4"/>
       <c r="H100" s="4"/>
     </row>
-    <row r="101" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F101" s="3">
         <v>44922</v>
       </c>
       <c r="G101" s="4"/>
       <c r="H101" s="4"/>
     </row>
-    <row r="102" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F102" s="3">
         <v>44923</v>
       </c>
       <c r="G102" s="4"/>
       <c r="H102" s="4"/>
     </row>
-    <row r="103" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F103" s="3">
         <v>44924</v>
       </c>
       <c r="G103" s="4"/>
       <c r="H103" s="4"/>
     </row>
-    <row r="104" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F104" s="3">
         <v>44925</v>
       </c>
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
     </row>
-    <row r="105" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F105" s="3">
         <v>44926</v>
       </c>
       <c r="G105" s="4"/>
       <c r="H105" s="4"/>
     </row>
-    <row r="106" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F106" s="3">
         <v>44927</v>
       </c>
       <c r="G106" s="4"/>
       <c r="H106" s="4"/>
     </row>
-    <row r="107" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F107" s="3">
         <v>44928</v>
       </c>
       <c r="G107" s="4"/>
       <c r="H107" s="4"/>
     </row>
-    <row r="108" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F108" s="3">
         <v>44929</v>
       </c>
       <c r="G108" s="4"/>
       <c r="H108" s="4"/>
     </row>
-    <row r="109" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F109" s="3">
         <v>44930</v>
       </c>
       <c r="G109" s="4"/>
       <c r="H109" s="4"/>
     </row>
-    <row r="110" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F110" s="3">
         <v>44931</v>
       </c>
       <c r="G110" s="4"/>
       <c r="H110" s="4"/>
     </row>
-    <row r="111" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F111" s="3">
         <v>44932</v>
       </c>
       <c r="G111" s="4"/>
       <c r="H111" s="4"/>
     </row>
-    <row r="112" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="6:10" x14ac:dyDescent="0.3">
       <c r="F112" s="3">
         <v>44933</v>
       </c>
@@ -2953,38 +3052,38 @@
       <c r="F138" s="3"/>
     </row>
     <row r="139" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E139" s="7" t="s">
+      <c r="E139" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F139" s="7"/>
-      <c r="G139" s="8">
+      <c r="F139" s="8"/>
+      <c r="G139" s="6">
         <f>SUM(G5,G5:G137)</f>
-        <v>38.049999999999997</v>
-      </c>
-      <c r="H139" s="8">
+        <v>50.05</v>
+      </c>
+      <c r="H139" s="6">
         <f>SUM(H5,H6:H138)</f>
-        <v>29.349999999999998</v>
-      </c>
-      <c r="I139" s="8">
+        <v>39.599999999999994</v>
+      </c>
+      <c r="I139" s="6">
         <f>SUM(I5,I6:I138)</f>
-        <v>31.75</v>
-      </c>
-      <c r="J139" s="8">
+        <v>37.5</v>
+      </c>
+      <c r="J139" s="6">
         <f>SUM(J5,J6:J138)</f>
-        <v>53.85</v>
-      </c>
-      <c r="L139" s="8" t="s">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="L139" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="140" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E140" s="7"/>
-      <c r="F140" s="7"/>
-      <c r="G140" s="8"/>
-      <c r="H140" s="8"/>
-      <c r="I140" s="8"/>
-      <c r="J140" s="8"/>
-      <c r="L140" s="8"/>
+      <c r="E140" s="8"/>
+      <c r="F140" s="8"/>
+      <c r="G140" s="6"/>
+      <c r="H140" s="6"/>
+      <c r="I140" s="6"/>
+      <c r="J140" s="6"/>
+      <c r="L140" s="6"/>
     </row>
     <row r="141" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E141" s="9" t="s">
@@ -3003,50 +3102,45 @@
       <c r="J141" s="5">
         <v>15.625</v>
       </c>
-      <c r="L141" s="8"/>
+      <c r="L141" s="6"/>
     </row>
     <row r="142" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E142" s="8" t="s">
+      <c r="E142" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F142" s="8"/>
-      <c r="G142" s="8">
+      <c r="F142" s="6"/>
+      <c r="G142" s="6">
         <f>PRODUCT(G139,G141)</f>
-        <v>594.53125</v>
-      </c>
-      <c r="H142" s="8">
+        <v>782.03125</v>
+      </c>
+      <c r="H142" s="6">
         <f>PRODUCT(H139,H141)</f>
-        <v>458.59374999999994</v>
-      </c>
-      <c r="I142" s="8">
+        <v>618.74999999999989</v>
+      </c>
+      <c r="I142" s="6">
         <f t="shared" ref="I142:J142" si="0">PRODUCT(I139,I141)</f>
-        <v>496.09375</v>
-      </c>
-      <c r="J142" s="8">
+        <v>585.9375</v>
+      </c>
+      <c r="J142" s="6">
         <f t="shared" si="0"/>
-        <v>841.40625</v>
-      </c>
-      <c r="L142" s="8">
+        <v>1071.875</v>
+      </c>
+      <c r="L142" s="6">
         <f>SUM(G142:J143)</f>
-        <v>2390.625</v>
+        <v>3058.59375</v>
       </c>
     </row>
     <row r="143" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="E143" s="8"/>
-      <c r="F143" s="8"/>
-      <c r="G143" s="8"/>
-      <c r="H143" s="8"/>
-      <c r="I143" s="8"/>
-      <c r="J143" s="8"/>
-      <c r="L143" s="8"/>
+      <c r="E143" s="6"/>
+      <c r="F143" s="6"/>
+      <c r="G143" s="6"/>
+      <c r="H143" s="6"/>
+      <c r="I143" s="6"/>
+      <c r="J143" s="6"/>
+      <c r="L143" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="L139:L141"/>
-    <mergeCell ref="L142:L143"/>
-    <mergeCell ref="I139:I140"/>
-    <mergeCell ref="J139:J140"/>
-    <mergeCell ref="J142:J143"/>
     <mergeCell ref="F2:I3"/>
     <mergeCell ref="E139:F140"/>
     <mergeCell ref="G139:G140"/>
@@ -3056,6 +3150,11 @@
     <mergeCell ref="H142:H143"/>
     <mergeCell ref="E141:F141"/>
     <mergeCell ref="I142:I143"/>
+    <mergeCell ref="L139:L141"/>
+    <mergeCell ref="L142:L143"/>
+    <mergeCell ref="I139:I140"/>
+    <mergeCell ref="J139:J140"/>
+    <mergeCell ref="J142:J143"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>